<commit_message>
Updated file excel lộ trình + chia task
Sơn
</commit_message>
<xml_diff>
--- a/Plan_project.xlsx
+++ b/Plan_project.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>Deadline:</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Cài đặt thuật toán Apriori và Demo một thuật toán</t>
   </si>
   <si>
-    <t xml:space="preserve">Thêm cơ sở dữ liệu sử dụng Entity CodeFirst </t>
-  </si>
-  <si>
     <t>Có một số dòng dữ liệu Demo</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Chia bảng sau</t>
   </si>
   <si>
-    <t>Có thể áp dụng cho mọi bảng</t>
-  </si>
-  <si>
     <t xml:space="preserve">Áp dụng Webservice, WebAPI, Angular </t>
   </si>
   <si>
@@ -280,6 +274,15 @@
   </si>
   <si>
     <t>https://github.com/trandinhson2112cntt/Web_Datamining_Hutech</t>
+  </si>
+  <si>
+    <t>Database + CodeFirst</t>
+  </si>
+  <si>
+    <t>Import dữ liệu từ excel Có thể áp dụng cho mọi bảng</t>
+  </si>
+  <si>
+    <t>Xây dựng database + design pattern</t>
   </si>
 </sst>
 </file>
@@ -290,7 +293,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +412,12 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -492,7 +501,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -589,6 +598,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -601,8 +614,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1218,8 +1230,8 @@
   </sheetPr>
   <dimension ref="B1:G70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1249,51 +1261,51 @@
       </c>
     </row>
     <row r="3" spans="2:7" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="33"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="29"/>
       <c r="G3" s="31" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="34">
+      <c r="B4" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="36">
         <v>43450</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="29"/>
       <c r="G4" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
       <c r="G5" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="5"/>
       <c r="G6" s="31" t="s">
         <v>16</v>
@@ -1316,12 +1328,12 @@
         <v>11</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>10</v>
@@ -1335,8 +1347,8 @@
       <c r="F8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>83</v>
+      <c r="G8" s="32" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
@@ -1344,13 +1356,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>17</v>
@@ -1362,13 +1374,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>17</v>
@@ -1380,13 +1392,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>17</v>
@@ -1395,15 +1407,17 @@
     </row>
     <row r="12" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9">
-        <v>0</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>84</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="12"/>
+      <c r="E12" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="F12" s="13" t="s">
         <v>17</v>
       </c>
@@ -1414,11 +1428,11 @@
         <v>0</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="10"/>
@@ -1426,23 +1440,23 @@
     <row r="14" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="14"/>
       <c r="C14" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="17"/>
       <c r="F14" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="15"/>
     </row>
     <row r="15" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19"/>
       <c r="C15" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1452,16 +1466,16 @@
         <v>0</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -1470,16 +1484,16 @@
         <v>0</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -1488,16 +1502,16 @@
         <v>0</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G18" s="10"/>
     </row>
@@ -1506,16 +1520,16 @@
         <v>0</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -1524,16 +1538,16 @@
         <v>0</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G20" s="10"/>
     </row>
@@ -1542,28 +1556,28 @@
         <v>0</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>44</v>
       </c>
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="14"/>
       <c r="C22" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="17"/>
       <c r="F22" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G22" s="15"/>
     </row>
@@ -1572,23 +1586,23 @@
         <v>0</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="9"/>
       <c r="C24" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D24" s="24"/>
       <c r="E24" s="10"/>
@@ -1600,16 +1614,16 @@
         <v>0</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G25" s="10"/>
     </row>
@@ -1618,16 +1632,16 @@
         <v>0</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G26" s="10"/>
     </row>
@@ -1636,16 +1650,16 @@
         <v>0</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="G27" s="10"/>
     </row>
@@ -1654,28 +1668,28 @@
         <v>0</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>55</v>
       </c>
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="14"/>
       <c r="C29" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="17"/>
       <c r="F29" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G29" s="15"/>
     </row>
@@ -1684,28 +1698,28 @@
         <v>0</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G30" s="10"/>
     </row>
     <row r="31" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="9"/>
       <c r="C31" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="10"/>
       <c r="F31" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G31" s="10"/>
     </row>
@@ -1714,16 +1728,16 @@
         <v>0</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G32" s="10"/>
     </row>
@@ -1732,27 +1746,27 @@
         <v>0</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="25"/>
       <c r="C34" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D34" s="25"/>
       <c r="E34" s="25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
@@ -1762,16 +1776,16 @@
         <v>0</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -1780,28 +1794,28 @@
         <v>0</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G36" s="10"/>
     </row>
     <row r="37" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="9"/>
       <c r="C37" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="10"/>
       <c r="F37" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G37" s="10"/>
     </row>
@@ -1810,14 +1824,14 @@
         <v>0</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G38" s="10"/>
     </row>
@@ -1826,26 +1840,26 @@
         <v>0</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G39" s="10"/>
     </row>
     <row r="40" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="14"/>
       <c r="C40" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="17"/>
       <c r="F40" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G40" s="15"/>
     </row>
@@ -1854,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>5</v>
@@ -1868,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>8</v>
@@ -1882,10 +1896,10 @@
         <v>0</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="13"/>
@@ -1896,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D44" s="24"/>
       <c r="E44" s="10"/>
@@ -1908,7 +1922,7 @@
         <v>0</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D45" s="24"/>
       <c r="E45" s="10"/>
@@ -1920,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D46" s="24"/>
       <c r="E46" s="10"/>
@@ -1930,12 +1944,12 @@
     <row r="47" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="14"/>
       <c r="C47" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="17"/>
       <c r="F47" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G47" s="10"/>
     </row>

</xml_diff>

<commit_message>
Update báo cáo tiến độ lần 1
</commit_message>
<xml_diff>
--- a/Plan_project.xlsx
+++ b/Plan_project.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>Deadline:</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Xây dựng database + design pattern</t>
+  </si>
+  <si>
+    <t>http://localhost:52360/api/luatxettuyen/create?sup=30&amp;&amp;con=50</t>
   </si>
 </sst>
 </file>
@@ -601,6 +604,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -613,9 +619,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1230,8 +1233,8 @@
   </sheetPr>
   <dimension ref="B1:G70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1261,51 +1264,51 @@
       </c>
     </row>
     <row r="3" spans="2:7" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="35" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="35"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="29"/>
       <c r="G3" s="31" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36">
+      <c r="B4" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="37">
         <v>43450</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="29"/>
       <c r="G4" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
       <c r="G5" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="5"/>
       <c r="G6" s="31" t="s">
         <v>16</v>
@@ -1353,7 +1356,7 @@
     </row>
     <row r="9" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>21</v>
@@ -1367,11 +1370,13 @@
       <c r="F9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="10"/>
+      <c r="G9" s="32" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>23</v>
@@ -1389,7 +1394,7 @@
     </row>
     <row r="11" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="9">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>24</v>
@@ -1409,7 +1414,7 @@
       <c r="B12" s="9">
         <v>1</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="33" t="s">
         <v>84</v>
       </c>
       <c r="D12" s="11" t="s">
@@ -1425,7 +1430,7 @@
     </row>
     <row r="13" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>79</v>
@@ -2045,15 +2050,16 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1"/>
+    <hyperlink ref="G9" r:id="rId2"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.25" footer="0.25"/>
-  <pageSetup scale="45" fitToHeight="0" orientation="portrait" r:id="rId2"/>
+  <pageSetup scale="45" fitToHeight="0" orientation="portrait" r:id="rId3"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cài đặt lại và đổi tên mấy cái luật xét tuyển => luật Xong: api/luathoctap/create Khoa => Môn học vượt
</commit_message>
<xml_diff>
--- a/Plan_project.xlsx
+++ b/Plan_project.xlsx
@@ -1230,7 +1230,7 @@
   </sheetPr>
   <dimension ref="B1:G70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="9" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>21</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="10" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>23</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="13" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="9">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>77</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="16" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>83</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="17" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>84</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="19" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="9">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Sửa biến _luatxetuyenservice => _luatservice Thêm api/luatxettuyen: Hình thức => Tỉnh
</commit_message>
<xml_diff>
--- a/Plan_project.xlsx
+++ b/Plan_project.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
   <si>
     <t>Deadline:</t>
   </si>
@@ -252,9 +252,6 @@
     <t>Sơn, Thịnh, Thành</t>
   </si>
   <si>
-    <t>Nghỉ ngơi</t>
-  </si>
-  <si>
     <t>12/11 - 26/11</t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t>Thêm xóa sửa liên quan tuyển sinh</t>
+  </si>
+  <si>
+    <t>Finished</t>
   </si>
 </sst>
 </file>
@@ -1230,8 +1230,8 @@
   </sheetPr>
   <dimension ref="B1:G70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1290,7 +1290,7 @@
     </row>
     <row r="5" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -1348,12 +1348,12 @@
         <v>17</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>21</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="10" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>23</v>
@@ -1410,13 +1410,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>17</v>
@@ -1425,20 +1425,22 @@
     </row>
     <row r="13" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
+      <c r="B14" s="14" t="s">
+        <v>84</v>
+      </c>
       <c r="C14" s="15" t="s">
         <v>29</v>
       </c>
@@ -1463,10 +1465,10 @@
     </row>
     <row r="16" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>5</v>
@@ -1481,10 +1483,10 @@
     </row>
     <row r="17" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>7</v>
@@ -1508,7 +1510,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>40</v>
@@ -1517,7 +1519,7 @@
     </row>
     <row r="19" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>34</v>
@@ -1570,7 +1572,9 @@
       <c r="G21" s="10"/>
     </row>
     <row r="22" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="14"/>
+      <c r="B22" s="14" t="s">
+        <v>84</v>
+      </c>
       <c r="C22" s="15" t="s">
         <v>29</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>54</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="10"/>
     </row>
@@ -1719,7 +1723,7 @@
       <c r="D31" s="24"/>
       <c r="E31" s="10"/>
       <c r="F31" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G31" s="10"/>
     </row>
@@ -1737,7 +1741,7 @@
         <v>56</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G32" s="10"/>
     </row>
@@ -1755,7 +1759,7 @@
         <v>67</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G33" s="10"/>
     </row>
@@ -1785,7 +1789,7 @@
         <v>60</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -1803,7 +1807,7 @@
         <v>62</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G36" s="10"/>
     </row>
@@ -1815,7 +1819,7 @@
       <c r="D37" s="24"/>
       <c r="E37" s="10"/>
       <c r="F37" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G37" s="10"/>
     </row>
@@ -1831,7 +1835,7 @@
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G38" s="10"/>
     </row>
@@ -1847,7 +1851,7 @@
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G39" s="10"/>
     </row>
@@ -1910,9 +1914,11 @@
         <v>0</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D44" s="24"/>
+        <v>72</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="E44" s="10"/>
       <c r="F44" s="13"/>
       <c r="G44" s="10"/>
@@ -1922,9 +1928,11 @@
         <v>0</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D45" s="24"/>
+        <v>72</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="E45" s="10"/>
       <c r="F45" s="13"/>
       <c r="G45" s="10"/>
@@ -1934,9 +1942,11 @@
         <v>0</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="24"/>
+        <v>72</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>73</v>
+      </c>
       <c r="E46" s="10"/>
       <c r="F46" s="13"/>
       <c r="G46" s="10"/>
@@ -1986,7 +1996,34 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B35:B39 B8:B14 B23:B28 B16:B21 B30:B33 B41:B46">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B40">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1995,33 +2032,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="dataBar" priority="4">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF92D050"/>
-      </dataBar>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="dataBar" priority="3">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF92D050"/>
-      </dataBar>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF92D050"/>
-      </dataBar>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Chỉnh sửa config api Thêm api/data/getallmonhoc va getallkhoa
</commit_message>
<xml_diff>
--- a/Plan_project.xlsx
+++ b/Plan_project.xlsx
@@ -24,6 +24,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <webPublishing codePage="1252"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -501,7 +502,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -603,6 +604,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1230,8 +1234,8 @@
   </sheetPr>
   <dimension ref="B1:G70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1261,51 +1265,51 @@
       </c>
     </row>
     <row r="3" spans="2:7" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="36"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="29"/>
       <c r="G3" s="31" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="30" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="37">
+      <c r="B4" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="38">
         <v>43450</v>
       </c>
-      <c r="E4" s="37"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="29"/>
       <c r="G4" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
       <c r="G5" s="31" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="5"/>
       <c r="G6" s="31" t="s">
         <v>16</v>
@@ -1769,7 +1773,7 @@
         <v>57</v>
       </c>
       <c r="D34" s="25"/>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="34" t="s">
         <v>58</v>
       </c>
       <c r="F34" s="27"/>

</xml_diff>

<commit_message>
Updated bảng phân công công việc
</commit_message>
<xml_diff>
--- a/Plan_project.xlsx
+++ b/Plan_project.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
   <si>
     <t>Deadline:</t>
   </si>
@@ -114,9 +114,6 @@
     <t>15/10</t>
   </si>
   <si>
-    <t>Trang ADMIN</t>
-  </si>
-  <si>
     <t>Báo cáo tiến độ</t>
   </si>
   <si>
@@ -204,30 +201,6 @@
     <t>Trang User</t>
   </si>
   <si>
-    <t>Angular (SPA)</t>
-  </si>
-  <si>
-    <t>Đăng nhập dựa trên MSSV</t>
-  </si>
-  <si>
-    <t>Đối với đối tượng về học tập</t>
-  </si>
-  <si>
-    <t>Đăng ký tài khoản</t>
-  </si>
-  <si>
-    <t>Đối với đối tượng tuyển sinh</t>
-  </si>
-  <si>
-    <t>Học tập</t>
-  </si>
-  <si>
-    <t>Luật học tập: Học vượt</t>
-  </si>
-  <si>
-    <t>Luật học tập: Học cải thiện</t>
-  </si>
-  <si>
     <t>Lưạ chọn bằng tay + mắt đối với những luật chưa được phù hợp</t>
   </si>
   <si>
@@ -240,12 +213,6 @@
     <t>10/12</t>
   </si>
   <si>
-    <t>Luật tuyển sinh:Nhập ngành muốn học</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luật tuyển sinh: Khảo sát điểm </t>
-  </si>
-  <si>
     <t>Chỉnh sửa bắt lỗi fix bug bổ sung</t>
   </si>
   <si>
@@ -270,9 +237,6 @@
     <t>Database + CodeFirst</t>
   </si>
   <si>
-    <t>Import dữ liệu từ excel Có thể áp dụng cho mọi bảng</t>
-  </si>
-  <si>
     <t>Xây dựng database + design pattern</t>
   </si>
   <si>
@@ -283,6 +247,51 @@
   </si>
   <si>
     <t>Finished</t>
+  </si>
+  <si>
+    <t>Trang Admin</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Hiển thị danh sách tất cả các luật</t>
+  </si>
+  <si>
+    <t>Import dữ liệu từ excel đối với các bảng điểm + môn học + điểm chi tiết + điểm tuyển sinh + hồ sơ + sinh viên</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>code bên phía Server</t>
+  </si>
+  <si>
+    <t>Dựa trên api create có sẵn</t>
+  </si>
+  <si>
+    <t>Triển khai các luật học tập</t>
+  </si>
+  <si>
+    <t>Triển khai các luật tuyển sinh</t>
+  </si>
+  <si>
+    <t>Dựa trên api getall có sẵn</t>
+  </si>
+  <si>
+    <t>Sử dụng tất cả các luật học tập + tuyển sinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viết thểm 1 api post để thêm dữ liệu như điểm môn học,tên thí sinh,tỉnh thành phố vào bảng hồ sơ + điểm </t>
+  </si>
+  <si>
+    <t>Tạo và hiển thị danh sách tất cả các luật</t>
+  </si>
+  <si>
+    <t>Triển khai các luật cho phòng đào tạo</t>
   </si>
 </sst>
 </file>
@@ -293,7 +302,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,8 +427,36 @@
       <name val="Franklin Gothic Book"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FFFF0000"/>
+      <name val="Perpetua"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +493,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -501,7 +550,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -619,6 +668,33 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1231,10 +1307,10 @@
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G70"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1245,7 +1321,7 @@
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="53.625" customWidth="1"/>
     <col min="6" max="6" width="30.125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="48.625" customWidth="1"/>
+    <col min="7" max="7" width="51.375" customWidth="1"/>
     <col min="8" max="8" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1293,7 +1369,7 @@
     </row>
     <row r="5" spans="2:7" ht="28.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
@@ -1351,7 +1427,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="32" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
@@ -1392,13 +1468,13 @@
     </row>
     <row r="11" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>25</v>
@@ -1413,13 +1489,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>17</v>
@@ -1428,24 +1504,24 @@
     </row>
     <row r="13" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="9">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="12" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="10"/>
     </row>
     <row r="14" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="14" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="17"/>
@@ -1457,11 +1533,11 @@
     <row r="15" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="19"/>
       <c r="C15" s="20" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1471,16 +1547,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="10"/>
     </row>
@@ -1489,34 +1565,34 @@
         <v>1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" s="10"/>
     </row>
@@ -1528,92 +1604,92 @@
         <v>34</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>36</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="9">
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="9">
-        <v>1</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="24" t="s">
+      <c r="D22" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="15"/>
+      <c r="E22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="10"/>
     </row>
     <row r="23" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="9">
-        <v>1</v>
-      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="9"/>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
       <c r="C24" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="13"/>
+      <c r="D24" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
@@ -1621,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>5</v>
@@ -1630,7 +1706,7 @@
         <v>44</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="10"/>
     </row>
@@ -1642,17 +1718,17 @@
         <v>46</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="2:7" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="9">
         <v>1</v>
       </c>
@@ -1663,310 +1739,331 @@
         <v>7</v>
       </c>
       <c r="E27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="14"/>
+      <c r="C28" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="G28" s="41"/>
+    </row>
+    <row r="29" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="9"/>
+      <c r="C29" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="2:7" s="8" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="9">
+      <c r="D29" s="24"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="9">
         <v>1</v>
       </c>
-      <c r="C28" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="14"/>
-      <c r="C29" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="9">
+      <c r="C30" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="25"/>
+      <c r="C31" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="27"/>
+      <c r="G31" s="42"/>
+    </row>
+    <row r="32" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="9">
         <v>0</v>
       </c>
-      <c r="C30" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="9"/>
-      <c r="C31" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="2:7" s="1" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="9">
-        <v>1</v>
-      </c>
       <c r="C32" s="23" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="9">
         <v>0</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D33" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="52.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="9">
+        <v>0</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" s="13" t="s">
+      <c r="E34" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="44"/>
+      <c r="C35" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="46"/>
+      <c r="G35" s="48"/>
+    </row>
+    <row r="36" spans="1:7" ht="53.4" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A36" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="25"/>
-      <c r="C34" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-    </row>
-    <row r="35" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="9">
-        <v>0</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="9">
         <v>0</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="9">
+        <v>0</v>
+      </c>
       <c r="C37" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="24"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" s="10"/>
-    </row>
-    <row r="38" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G37" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="9">
         <v>0</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="F38" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="9">
         <v>0</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="F39" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="14"/>
       <c r="C40" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="17"/>
       <c r="F40" s="18" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G40" s="15"/>
     </row>
-    <row r="41" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="9">
         <v>0</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="13"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="9">
         <v>0</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="13"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B43" s="9">
         <v>0</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="13"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B44" s="9">
         <v>0</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="13"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="9">
         <v>0</v>
       </c>
       <c r="C45" s="23" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="13"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="9">
         <v>0</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E46" s="10"/>
       <c r="F46" s="13"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="14"/>
       <c r="C47" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D47" s="16"/>
       <c r="E47" s="17"/>
       <c r="F47" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G47" s="10"/>
-    </row>
-    <row r="48" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
+        <v>60</v>
+      </c>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="48" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="50" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="51" ht="33" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1998,8 +2095,8 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B35:B39 B8:B14 B23:B28 B16:B21 B30:B33 B41:B46">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="B28">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2007,7 +2104,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
+  <conditionalFormatting sqref="B40">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
@@ -2016,7 +2113,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
+  <conditionalFormatting sqref="B47">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -2025,7 +2122,7 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47">
+  <conditionalFormatting sqref="B21">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -2034,7 +2131,16 @@
       </dataBar>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
+  <conditionalFormatting sqref="B41:B46 B8:B14 B22:B27 B16:B20 B29:B30 B36:B38 B32:B34">
+    <cfRule type="dataBar" priority="11">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF92D050"/>
+      </dataBar>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>

</xml_diff>